<commit_message>
updated the experiment template
</commit_message>
<xml_diff>
--- a/article_28_question_answer_pairs.xlsx
+++ b/article_28_question_answer_pairs.xlsx
@@ -13,17 +13,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1737624968" val="1222" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1737624968" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1737624968" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1737624968"/>
+      <pm:revision xmlns:pm="smNativeData" day="1737627722" val="1222" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1737627722" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1737627722" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1737627722"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>Search for explicit clauses stating that the financial entity retains full responsibility for DORA compliance. Look specifically for:
  - Clear statements of retained responsibility
@@ -42,6 +42,9 @@
  • References to specific financial services laws
  ▪ 
 Follow-up if Missing: Recommend adding explicit clause covering retention of regulatory responsibilities for all applicable financial services laws.</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
   <si>
     <t>Search for provisions requiring senior management or board approval of ICT service agreements. Look for:
@@ -108,7 +111,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1737624968" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1737627722" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -123,7 +126,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1737624968" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1737627722" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -145,7 +148,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1737624968" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1737627722" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -167,7 +170,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1737624968"/>
+          <pm:border xmlns:pm="smNativeData" id="1737627722"/>
         </ext>
       </extLst>
     </border>
@@ -186,7 +189,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1737624968"/>
+          <pm:border xmlns:pm="smNativeData" id="1737627722"/>
         </ext>
       </extLst>
     </border>
@@ -206,7 +209,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1737624968" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1737627722" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
     </ext>
@@ -472,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.40"/>
@@ -491,41 +494,59 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1737624968" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1737627722" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -534,14 +555,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1737624968" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1737624968" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1737627722" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1737627722" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1737624968" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1737627722" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>